<commit_message>
making processing and analysis knit prove and minor changes
</commit_message>
<xml_diff>
--- a/Week 10/implicit evaluations study/data/processed/data_processed_codebook.xlsx
+++ b/Week 10/implicit evaluations study/data/processed/data_processed_codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studium\Master\3 HS 23\Methods seminar Improving the credibility of future research\Methods-seminar digital-project-managment\dpm-assignments\Week 10\implicit evaluations study\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698CAB87-DDC5-4336-B050-FABB58719C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE39E608-0470-47F2-ABC5-2530856A2610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -468,7 +468,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>